<commit_message>
backlog finalizado e alterações game
</commit_message>
<xml_diff>
--- a/backlog.xlsx
+++ b/backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorge\Desktop\projeto pessoal\Projeto-Individual\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A18711A8-3271-4BB4-8EC0-58A7668836C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D07B7136-2A33-4CA1-AA23-61A5BE84397A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{31297882-7B3D-4F90-B3D3-D07F0AF0B13D}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="85">
   <si>
     <t>PROJETO INDIVIDUAL - BACKLOG</t>
   </si>
@@ -289,6 +289,9 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>FINALIZADO</t>
   </si>
 </sst>
 </file>
@@ -399,7 +402,27 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -813,8 +836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3300CF5-4A63-4592-BC70-E1407BE78AF5}">
   <dimension ref="A1:R31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B12" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -822,7 +845,7 @@
     <col min="1" max="1" width="39" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="74.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" customWidth="1"/>
     <col min="8" max="8" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -882,14 +905,16 @@
         <v>5</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="G3" s="3"/>
+        <v>84</v>
+      </c>
+      <c r="G3" s="3">
+        <v>1</v>
+      </c>
       <c r="H3" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -906,15 +931,17 @@
         <f>IF(D4="P",5,IF(D4="PP",3,IF(D4="M",8,IF(D4="G",13,IF(D4="GG",21,"")))))</f>
         <v>8</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G4" s="4"/>
+      <c r="F4" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G4" s="4">
+        <v>1</v>
+      </c>
       <c r="H4" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>50</v>
       </c>
@@ -931,15 +958,17 @@
         <f t="shared" ref="E5:E31" si="0">IF(D5="P",5,IF(D5="PP",3,IF(D5="M",8,IF(D5="G",13,IF(D5="GG",21,"")))))</f>
         <v>3</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G5" s="4"/>
+      <c r="F5" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G5" s="4">
+        <v>1</v>
+      </c>
       <c r="H5" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
@@ -956,15 +985,17 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G6" s="4"/>
+      <c r="F6" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G6" s="4">
+        <v>1</v>
+      </c>
       <c r="H6" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>77</v>
       </c>
@@ -981,10 +1012,12 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="F7" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G7" s="4"/>
+      <c r="F7" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G7" s="4">
+        <v>1</v>
+      </c>
       <c r="H7" s="4">
         <v>1</v>
       </c>
@@ -1006,15 +1039,17 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="F8" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G8" s="4"/>
+      <c r="F8" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G8" s="4">
+        <v>2</v>
+      </c>
       <c r="H8" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>79</v>
       </c>
@@ -1031,10 +1066,12 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="F9" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G9" s="4"/>
+      <c r="F9" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G9" s="4">
+        <v>2</v>
+      </c>
       <c r="H9" s="4">
         <v>1</v>
       </c>
@@ -1042,7 +1079,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
@@ -1059,15 +1096,17 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="F10" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G10" s="4"/>
+      <c r="F10" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G10" s="4">
+        <v>2</v>
+      </c>
       <c r="H10" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
@@ -1084,15 +1123,17 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="F11" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G11" s="4"/>
+      <c r="F11" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G11" s="4">
+        <v>2</v>
+      </c>
       <c r="H11" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
@@ -1109,15 +1150,17 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="F12" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G12" s="4"/>
+      <c r="F12" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G12" s="4">
+        <v>2</v>
+      </c>
       <c r="H12" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>7</v>
       </c>
@@ -1134,15 +1177,17 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="F13" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G13" s="4"/>
+      <c r="F13" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G13" s="4">
+        <v>3</v>
+      </c>
       <c r="H13" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>8</v>
       </c>
@@ -1159,10 +1204,12 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="F14" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G14" s="4"/>
+      <c r="F14" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G14" s="4">
+        <v>3</v>
+      </c>
       <c r="H14" s="4">
         <v>1</v>
       </c>
@@ -1184,10 +1231,12 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="F15" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G15" s="4"/>
+      <c r="F15" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G15" s="4">
+        <v>3</v>
+      </c>
       <c r="H15" s="4">
         <v>2</v>
       </c>
@@ -1209,15 +1258,17 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="F16" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G16" s="4"/>
+      <c r="F16" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G16" s="4">
+        <v>4</v>
+      </c>
       <c r="H16" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>26</v>
       </c>
@@ -1234,10 +1285,12 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="F17" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G17" s="4"/>
+      <c r="F17" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G17" s="4">
+        <v>4</v>
+      </c>
       <c r="H17" s="4">
         <v>2</v>
       </c>
@@ -1259,10 +1312,12 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="F18" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G18" s="4"/>
+      <c r="F18" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G18" s="4">
+        <v>4</v>
+      </c>
       <c r="H18" s="4">
         <v>3</v>
       </c>
@@ -1270,7 +1325,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>30</v>
       </c>
@@ -1287,8 +1342,8 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="F19" s="4" t="s">
-        <v>60</v>
+      <c r="F19" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="G19" s="4"/>
       <c r="H19" s="4">
@@ -1315,10 +1370,12 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="F20" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G20" s="4"/>
+      <c r="F20" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G20" s="4">
+        <v>1</v>
+      </c>
       <c r="H20" s="4">
         <v>1</v>
       </c>
@@ -1347,10 +1404,12 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="F21" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G21" s="4"/>
+      <c r="F21" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G21" s="4">
+        <v>1</v>
+      </c>
       <c r="H21" s="4">
         <v>1</v>
       </c>
@@ -1375,10 +1434,12 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="F22" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G22" s="4"/>
+      <c r="F22" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G22" s="4">
+        <v>1</v>
+      </c>
       <c r="H22" s="4">
         <v>2</v>
       </c>
@@ -1389,7 +1450,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>37</v>
       </c>
@@ -1406,10 +1467,12 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="F23" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G23" s="4"/>
+      <c r="F23" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G23" s="4">
+        <v>1</v>
+      </c>
       <c r="H23" s="4">
         <v>2</v>
       </c>
@@ -1437,10 +1500,12 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="F24" s="4" t="s">
+      <c r="F24" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="G24" s="4"/>
+      <c r="G24" s="4">
+        <v>4</v>
+      </c>
       <c r="H24" s="4">
         <v>2</v>
       </c>
@@ -1465,15 +1530,17 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="F25" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G25" s="4"/>
+      <c r="F25" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G25" s="4">
+        <v>3</v>
+      </c>
       <c r="H25" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>12</v>
       </c>
@@ -1490,15 +1557,17 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="F26" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G26" s="4"/>
+      <c r="F26" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G26" s="4">
+        <v>2</v>
+      </c>
       <c r="H26" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>13</v>
       </c>
@@ -1515,15 +1584,17 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="F27" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G27" s="4"/>
+      <c r="F27" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G27" s="4">
+        <v>2</v>
+      </c>
       <c r="H27" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>44</v>
       </c>
@@ -1540,15 +1611,17 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="F28" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G28" s="4"/>
+      <c r="F28" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G28" s="4">
+        <v>3</v>
+      </c>
       <c r="H28" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>14</v>
       </c>
@@ -1565,15 +1638,17 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="F29" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G29" s="4"/>
+      <c r="F29" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G29" s="4">
+        <v>4</v>
+      </c>
       <c r="H29" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>15</v>
       </c>
@@ -1590,15 +1665,17 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="F30" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G30" s="4"/>
+      <c r="F30" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G30" s="4">
+        <v>1</v>
+      </c>
       <c r="H30" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>48</v>
       </c>
@@ -1615,10 +1692,12 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="F31" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G31" s="4"/>
+      <c r="F31" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G31" s="4">
+        <v>2</v>
+      </c>
       <c r="H31" s="4">
         <v>3</v>
       </c>
@@ -1628,8 +1707,13 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <conditionalFormatting sqref="G2:H3 F2:F1048576">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>"PENDENTE"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3:F31">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>"PENDENTE"</formula>
+      <formula>"FINALIZADO"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>